<commit_message>
Added photos from last 3 months, since Jan 24, 2019.
</commit_message>
<xml_diff>
--- a/images/iMaGeUpLoAdErMaGiXpRo.xlsx
+++ b/images/iMaGeUpLoAdErMaGiXpRo.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
   <si>
     <r>
       <t xml:space="preserve">" </t>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>7R305915web.jpg</t>
+  </si>
+  <si>
+    <t>How to use: Paste file names into column B, then copy column D into code</t>
   </si>
 </sst>
 </file>
@@ -596,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -610,19 +613,9 @@
     <col min="4" max="4" width="44.1640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="3" t="str">
-        <f>CONCATENATE(A1,B1,C1)</f>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305777web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -630,14 +623,14 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="3" t="str">
-        <f t="shared" ref="D2:D31" si="0">CONCATENATE(A2,B2,C2)</f>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305711web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
+        <f>CONCATENATE(A2,B2,C2)</f>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305777web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -645,14 +638,14 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305682-editplainweb.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
+        <f t="shared" ref="D3:D17" si="0">CONCATENATE(A3,B3,C3)</f>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305711web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -660,14 +653,14 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305745web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305682-editplainweb.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -675,14 +668,14 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305784web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305745web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -690,14 +683,14 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305685web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305784web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -705,14 +698,14 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305836web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305685web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -720,14 +713,14 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305866web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305836web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -735,14 +728,14 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305699web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305866web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -750,14 +743,14 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305857web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305699web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -765,14 +758,14 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305804web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305857web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -780,14 +773,14 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305813web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305804web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -795,14 +788,14 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305702web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305813web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -810,14 +803,14 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305782web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305702web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -825,14 +818,14 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305843web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305782web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -840,75 +833,90 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305843web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="3" t="str">
+      <c r="C17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3" t="str">
         <f t="shared" si="0"/>
         <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California/7R305915web.jpg" alt="Tahoe Sunny Forest Glowing through Snow, CA" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="C32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added photos to portraits, bay area, DC, and Berkeley
</commit_message>
<xml_diff>
--- a/images/iMaGeUpLoAdErMaGiXpRo.xlsx
+++ b/images/iMaGeUpLoAdErMaGiXpRo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcamozzo/Desktop/Danny's Stuff/Work/Development/Projects/Photo Website/dcamo001.github.io/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5DC02C-D4FE-F04E-ACBA-86E3C757A893}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD89330-8205-9846-BCB9-8FDCF63093A0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5420" yWindow="460" windowWidth="28440" windowHeight="22540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,177 +33,257 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="58">
   <si>
     <t>How to use: Paste file names into column B, then copy column D into code</t>
   </si>
   <si>
-    <t>7R302502web.jpg</t>
-  </si>
-  <si>
-    <t>7R302503web.jpg</t>
-  </si>
-  <si>
-    <t>7R302511web.jpg</t>
-  </si>
-  <si>
-    <t>7R302512web.jpg</t>
-  </si>
-  <si>
-    <t>7R302514web.jpg</t>
-  </si>
-  <si>
-    <t>7R302515web.jpg</t>
-  </si>
-  <si>
-    <t>7R302518web.jpg</t>
-  </si>
-  <si>
-    <t>7R302520web.jpg</t>
-  </si>
-  <si>
-    <t>7R302529web.jpg</t>
-  </si>
-  <si>
-    <t>7R302530web.jpg</t>
-  </si>
-  <si>
-    <t>7R302537web.jpg</t>
-  </si>
-  <si>
-    <t>7R302543web.jpg</t>
-  </si>
-  <si>
-    <t>7R302551web.jpg</t>
-  </si>
-  <si>
-    <t>7R302557web.jpg</t>
-  </si>
-  <si>
-    <t>7R302560web.jpg</t>
-  </si>
-  <si>
-    <t>7R302574web.jpg</t>
-  </si>
-  <si>
-    <t>7R302580web.jpg</t>
-  </si>
-  <si>
-    <t>7R302583web.jpg</t>
-  </si>
-  <si>
-    <t>7R302608web.jpg</t>
-  </si>
-  <si>
-    <t>7R302610web.jpg</t>
-  </si>
-  <si>
-    <t>7R302620web.jpg</t>
-  </si>
-  <si>
-    <t>7R302622web.jpg</t>
-  </si>
-  <si>
-    <t>7R302624web.jpg</t>
-  </si>
-  <si>
-    <t>7R302629web.jpg</t>
-  </si>
-  <si>
-    <t>7R302633web.jpg</t>
-  </si>
-  <si>
-    <t>7R302636web.jpg</t>
-  </si>
-  <si>
-    <t>7R302639web.jpg</t>
-  </si>
-  <si>
-    <t>7R302644web.jpg</t>
-  </si>
-  <si>
-    <t>7R302649web.jpg</t>
-  </si>
-  <si>
-    <t>7R302652web.jpg</t>
-  </si>
-  <si>
-    <t>7R302684web.jpg</t>
-  </si>
-  <si>
-    <t>7R302694web.jpg</t>
-  </si>
-  <si>
-    <t>7R302701web.jpg</t>
-  </si>
-  <si>
-    <t>7R302710web.jpg</t>
-  </si>
-  <si>
-    <t>7R302717web.jpg</t>
-  </si>
-  <si>
-    <t>7R302721web.jpg</t>
-  </si>
-  <si>
-    <t>7R302727web.jpg</t>
-  </si>
-  <si>
-    <t>7R302731web.jpg</t>
-  </si>
-  <si>
-    <t>7R302735web.jpg</t>
-  </si>
-  <si>
-    <t>7R302746web.jpg</t>
-  </si>
-  <si>
-    <t>7R302754web.jpg</t>
-  </si>
-  <si>
-    <t>7R302761web.jpg</t>
-  </si>
-  <si>
-    <t>7R302762web.jpg</t>
-  </si>
-  <si>
-    <t>7R302765web.jpg</t>
-  </si>
-  <si>
-    <t>7R302767web.jpg</t>
-  </si>
-  <si>
-    <t>7R302774web.jpg</t>
-  </si>
-  <si>
-    <t>7R302783web.jpg</t>
-  </si>
-  <si>
-    <t>7R302802web.jpg</t>
-  </si>
-  <si>
-    <t>7R302803web.jpg</t>
-  </si>
-  <si>
-    <t>7R302819web.jpg</t>
-  </si>
-  <si>
-    <t>7R302828web.jpg</t>
-  </si>
-  <si>
-    <t>7R302837web.jpg</t>
-  </si>
-  <si>
-    <t>7R302839web.jpg</t>
-  </si>
-  <si>
-    <t>7R302848web.jpg</t>
-  </si>
-  <si>
-    <t>7R302850web.jpg</t>
-  </si>
-  <si>
-    <t>7R302862web.jpg</t>
+    <t>7R305417web.jpg</t>
+  </si>
+  <si>
+    <t>7R305592web.jpg</t>
+  </si>
+  <si>
+    <t>7R305589web.jpg</t>
+  </si>
+  <si>
+    <t>7R305588-2web.jpg</t>
+  </si>
+  <si>
+    <t>7R305588-1web.jpg</t>
+  </si>
+  <si>
+    <t>7R305587web.jpg</t>
+  </si>
+  <si>
+    <t>7R305586web.jpg</t>
+  </si>
+  <si>
+    <t>7R305585web.jpg</t>
+  </si>
+  <si>
+    <t>7R305579web.jpg</t>
+  </si>
+  <si>
+    <t>7R305578web.jpg</t>
+  </si>
+  <si>
+    <t>7R305566web.jpg</t>
+  </si>
+  <si>
+    <t>7R305564-Panoweb.jpg</t>
+  </si>
+  <si>
+    <t>7R305563web.jpg</t>
+  </si>
+  <si>
+    <t>7R305556web.jpg</t>
+  </si>
+  <si>
+    <t>7R305554web.jpg</t>
+  </si>
+  <si>
+    <t>7R305552web.jpg</t>
+  </si>
+  <si>
+    <t>7R305544web.jpg</t>
+  </si>
+  <si>
+    <t>7R305543web.jpg</t>
+  </si>
+  <si>
+    <t>7R305522web.jpg</t>
+  </si>
+  <si>
+    <t>7R305521web.jpg</t>
+  </si>
+  <si>
+    <t>7R305501web.jpg</t>
+  </si>
+  <si>
+    <t>7R305498web.jpg</t>
+  </si>
+  <si>
+    <t>7R305489web.jpg</t>
+  </si>
+  <si>
+    <t>7R305487web.jpg</t>
+  </si>
+  <si>
+    <t>7R305484web.jpg</t>
+  </si>
+  <si>
+    <t>7R305477web.jpg</t>
+  </si>
+  <si>
+    <t>7R305476web.jpg</t>
+  </si>
+  <si>
+    <t>7R305474web.jpg</t>
+  </si>
+  <si>
+    <t>7R305470web.jpg</t>
+  </si>
+  <si>
+    <t>7R305467web.jpg</t>
+  </si>
+  <si>
+    <t>7R305457web.jpg</t>
+  </si>
+  <si>
+    <t>7R305449web.jpg</t>
+  </si>
+  <si>
+    <t>7R305437web.jpg</t>
+  </si>
+  <si>
+    <t>7R305429web.jpg</t>
+  </si>
+  <si>
+    <t>7R305427web.jpg</t>
+  </si>
+  <si>
+    <t>7R305425web.jpg</t>
+  </si>
+  <si>
+    <t>7R305422web.jpg</t>
+  </si>
+  <si>
+    <t>7R305248web.jpg</t>
+  </si>
+  <si>
+    <t>7R305247web.jpg</t>
+  </si>
+  <si>
+    <t>7R302501web.jpg</t>
+  </si>
+  <si>
+    <t>7R302498web.jpg</t>
+  </si>
+  <si>
+    <t>7R301870web.jpg</t>
+  </si>
+  <si>
+    <t>7R301319web.jpg</t>
+  </si>
+  <si>
+    <t>7R301317stackedweb.jpg</t>
+  </si>
+  <si>
+    <t>7R300794web.jpg</t>
+  </si>
+  <si>
+    <t>7R300790web.jpg</t>
+  </si>
+  <si>
+    <t>7R300170web.jpg</t>
+  </si>
+  <si>
+    <t>7R300163web.jpg</t>
+  </si>
+  <si>
+    <t>7R300162web.jpg</t>
+  </si>
+  <si>
+    <t>7R300156web.jpg</t>
+  </si>
+  <si>
+    <t>7R300155web.jpg</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFEF596F"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>div</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFBBBBBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFBBBBBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF89CA78"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"masonryImage"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFBBBBBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt; &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>img</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFBBBBBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="7" tint="-0.249977111117893"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>src=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="9" tint="0.39997558519241921"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"images/California</t>
+    </r>
   </si>
   <si>
     <r>
@@ -225,7 +305,7 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>"Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco."</t>
+      <t>"Photos from the San Francisco Bay Area."</t>
     </r>
     <r>
       <rPr>
@@ -356,7 +436,21 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>"images/Events/RuthsTable</t>
+      <t>"images/Portraits</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFEF596F"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>div</t>
     </r>
     <r>
       <rPr>
@@ -365,7 +459,197 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>/</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFBBBBBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF89CA78"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"masonryImage"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFBBBBBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt; &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>img</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFBBBBBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="7" tint="-0.249977111117893"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>src=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="9" tint="0.39997558519241921"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"images/DCNoVA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="7" tint="-0.249977111117893"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>alt=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="9" tint="0.39997558519241921"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Photos from DC and the Eastern Shore of Maryland."</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF89CA78"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>/&gt;&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>div</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="7" tint="-0.249977111117893"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>alt=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="9" tint="0.39997558519241921"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Portraits from the San Francisco Bay Area."</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF89CA78"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>/&gt;&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>div</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
     </r>
   </si>
 </sst>
@@ -739,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D57"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43:D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -758,202 +1042,202 @@
     </row>
     <row r="2" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D2" s="3" t="str">
         <f>CONCATENATE(A2,B2,C2)</f>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302502web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305417web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f t="shared" ref="D3:D66" si="0">CONCATENATE(A3,B3,C3)</f>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302503web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <f t="shared" ref="D3:D57" si="0">CONCATENATE(A3,B3,C3)</f>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305592web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302511web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305589web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302512web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305588-2web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302514web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305588-1web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302515web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305587web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302518web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305586web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302520web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305585web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302529web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305579web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302530web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305578web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302537web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305566web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302543web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305564-Panoweb.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D14" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302551web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305563web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
@@ -963,12 +1247,12 @@
       </c>
       <c r="D15" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302557web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305556web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
@@ -978,87 +1262,87 @@
       </c>
       <c r="D16" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302560web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305554web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D17" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302574web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305552web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D18" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302580web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305544web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D19" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302583web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305543web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D20" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302608web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305522web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302610web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305521web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
@@ -1068,12 +1352,12 @@
       </c>
       <c r="D22" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302620web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305501web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
@@ -1083,57 +1367,57 @@
       </c>
       <c r="D23" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302622web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305498web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D24" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302624web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305489web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D25" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302629web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305487web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D26" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302633web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305484web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
@@ -1143,27 +1427,27 @@
       </c>
       <c r="D27" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302636web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305477web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D28" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302639web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305476web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
@@ -1173,27 +1457,27 @@
       </c>
       <c r="D29" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302644web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305474web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D30" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302649web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305470web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
@@ -1203,12 +1487,12 @@
       </c>
       <c r="D31" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302652web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305467web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B32" t="s">
         <v>31</v>
@@ -1218,27 +1502,27 @@
       </c>
       <c r="D32" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302684web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305457web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B33" t="s">
         <v>32</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D33" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302694web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305449web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B34" t="s">
         <v>33</v>
@@ -1248,12 +1532,12 @@
       </c>
       <c r="D34" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302701web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305437web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B35" t="s">
         <v>34</v>
@@ -1263,12 +1547,12 @@
       </c>
       <c r="D35" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302710web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305429web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B36" t="s">
         <v>35</v>
@@ -1278,12 +1562,12 @@
       </c>
       <c r="D36" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302717web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305427web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B37" t="s">
         <v>36</v>
@@ -1293,12 +1577,12 @@
       </c>
       <c r="D37" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302721web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305425web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B38" t="s">
         <v>37</v>
@@ -1308,293 +1592,238 @@
       </c>
       <c r="D38" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302727web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305422web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B39" t="s">
         <v>38</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D39" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302731web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305248web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B40" t="s">
         <v>39</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D40" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302735web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305247web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B41" t="s">
         <v>40</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D41" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302746web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R302501web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B42" t="s">
         <v>41</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D42" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302754web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R302498web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B43" t="s">
         <v>42</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D43" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302761web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/DCNoVA7R301870web.jpg" alt="Photos from DC and the Eastern Shore of Maryland." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B44" t="s">
         <v>43</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D44" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302762web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/DCNoVA7R301319web.jpg" alt="Photos from DC and the Eastern Shore of Maryland." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B45" t="s">
         <v>44</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D45" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302765web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/DCNoVA7R301317stackedweb.jpg" alt="Photos from DC and the Eastern Shore of Maryland." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B46" t="s">
         <v>45</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D46" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302767web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/DCNoVA7R300794web.jpg" alt="Photos from DC and the Eastern Shore of Maryland." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B47" t="s">
         <v>46</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D47" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302774web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/DCNoVA7R300790web.jpg" alt="Photos from DC and the Eastern Shore of Maryland." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B48" t="s">
         <v>47</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D48" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302783web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/DCNoVA7R300170web.jpg" alt="Photos from DC and the Eastern Shore of Maryland." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B49" t="s">
         <v>48</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D49" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302802web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/DCNoVA7R300163web.jpg" alt="Photos from DC and the Eastern Shore of Maryland." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B50" t="s">
         <v>49</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D50" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302803web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/DCNoVA7R300162web.jpg" alt="Photos from DC and the Eastern Shore of Maryland." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B51" t="s">
         <v>50</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D51" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302819web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/DCNoVA7R300156web.jpg" alt="Photos from DC and the Eastern Shore of Maryland." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B52" t="s">
         <v>51</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D52" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302828web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B53" t="s">
-        <v>52</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D53" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302837web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B54" t="s">
-        <v>53</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D54" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302839web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B55" t="s">
-        <v>54</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D55" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302848web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B56" t="s">
-        <v>55</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D56" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302850web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B57" t="s">
-        <v>56</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D57" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Events/RuthsTable/7R302862web.jpg" alt="Ruth's Table Gallery Opening in Mission Neighborhod In San Francisco." /&gt;&lt;/div&gt;</v>
-      </c>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/DCNoVA7R300155web.jpg" alt="Photos from DC and the Eastern Shore of Maryland." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="1"/>
+      <c r="C53" s="2"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="1"/>
+      <c r="C54" s="2"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="1"/>
+      <c r="C55" s="2"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
+      <c r="C56" s="2"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="1"/>
+      <c r="C57" s="2"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>

</xml_diff>

<commit_message>
Added new and newly edited photos in the Europe album, changed some description in the Prints and About pages
</commit_message>
<xml_diff>
--- a/images/iMaGeUpLoAdErMaGiXpRo.xlsx
+++ b/images/iMaGeUpLoAdErMaGiXpRo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcamozzo/Desktop/Danny's Stuff/Work/Development/Projects/Photo Website/dcamo001.github.io/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD89330-8205-9846-BCB9-8FDCF63093A0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8988EC0E-3D10-D348-9931-360FEFE6C07A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5420" yWindow="460" windowWidth="28440" windowHeight="22540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28440" windowHeight="22540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -33,162 +34,180 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="60">
   <si>
     <t>How to use: Paste file names into column B, then copy column D into code</t>
   </si>
   <si>
-    <t>7R305417web.jpg</t>
-  </si>
-  <si>
-    <t>7R305592web.jpg</t>
-  </si>
-  <si>
-    <t>7R305589web.jpg</t>
-  </si>
-  <si>
-    <t>7R305588-2web.jpg</t>
-  </si>
-  <si>
-    <t>7R305588-1web.jpg</t>
-  </si>
-  <si>
-    <t>7R305587web.jpg</t>
-  </si>
-  <si>
-    <t>7R305586web.jpg</t>
-  </si>
-  <si>
-    <t>7R305585web.jpg</t>
-  </si>
-  <si>
-    <t>7R305579web.jpg</t>
-  </si>
-  <si>
-    <t>7R305578web.jpg</t>
-  </si>
-  <si>
-    <t>7R305566web.jpg</t>
-  </si>
-  <si>
-    <t>7R305564-Panoweb.jpg</t>
-  </si>
-  <si>
-    <t>7R305563web.jpg</t>
-  </si>
-  <si>
-    <t>7R305556web.jpg</t>
-  </si>
-  <si>
-    <t>7R305554web.jpg</t>
-  </si>
-  <si>
-    <t>7R305552web.jpg</t>
-  </si>
-  <si>
-    <t>7R305544web.jpg</t>
-  </si>
-  <si>
-    <t>7R305543web.jpg</t>
-  </si>
-  <si>
-    <t>7R305522web.jpg</t>
-  </si>
-  <si>
-    <t>7R305521web.jpg</t>
-  </si>
-  <si>
-    <t>7R305501web.jpg</t>
-  </si>
-  <si>
-    <t>7R305498web.jpg</t>
-  </si>
-  <si>
-    <t>7R305489web.jpg</t>
-  </si>
-  <si>
-    <t>7R305487web.jpg</t>
-  </si>
-  <si>
-    <t>7R305484web.jpg</t>
-  </si>
-  <si>
-    <t>7R305477web.jpg</t>
-  </si>
-  <si>
-    <t>7R305476web.jpg</t>
-  </si>
-  <si>
-    <t>7R305474web.jpg</t>
-  </si>
-  <si>
-    <t>7R305470web.jpg</t>
-  </si>
-  <si>
-    <t>7R305467web.jpg</t>
-  </si>
-  <si>
-    <t>7R305457web.jpg</t>
-  </si>
-  <si>
-    <t>7R305449web.jpg</t>
-  </si>
-  <si>
-    <t>7R305437web.jpg</t>
-  </si>
-  <si>
-    <t>7R305429web.jpg</t>
-  </si>
-  <si>
-    <t>7R305427web.jpg</t>
-  </si>
-  <si>
-    <t>7R305425web.jpg</t>
-  </si>
-  <si>
-    <t>7R305422web.jpg</t>
-  </si>
-  <si>
-    <t>7R305248web.jpg</t>
-  </si>
-  <si>
-    <t>7R305247web.jpg</t>
-  </si>
-  <si>
-    <t>7R302501web.jpg</t>
-  </si>
-  <si>
-    <t>7R302498web.jpg</t>
-  </si>
-  <si>
-    <t>7R301870web.jpg</t>
-  </si>
-  <si>
-    <t>7R301319web.jpg</t>
-  </si>
-  <si>
-    <t>7R301317stackedweb.jpg</t>
-  </si>
-  <si>
-    <t>7R300794web.jpg</t>
-  </si>
-  <si>
-    <t>7R300790web.jpg</t>
-  </si>
-  <si>
-    <t>7R300170web.jpg</t>
-  </si>
-  <si>
-    <t>7R300163web.jpg</t>
-  </si>
-  <si>
-    <t>7R300162web.jpg</t>
-  </si>
-  <si>
-    <t>7R300156web.jpg</t>
-  </si>
-  <si>
-    <t>7R300155web.jpg</t>
+    <t>7R306533web.jpg</t>
+  </si>
+  <si>
+    <t>7R307103web.jpg</t>
+  </si>
+  <si>
+    <t>7R307046web.jpg</t>
+  </si>
+  <si>
+    <t>7R307044web.jpg</t>
+  </si>
+  <si>
+    <t>7R307035web.jpg</t>
+  </si>
+  <si>
+    <t>7R307033web.jpg</t>
+  </si>
+  <si>
+    <t>7R307031-Panoweb.jpg</t>
+  </si>
+  <si>
+    <t>7R307029web.jpg</t>
+  </si>
+  <si>
+    <t>7R307025web.jpg</t>
+  </si>
+  <si>
+    <t>7R307023web.jpg</t>
+  </si>
+  <si>
+    <t>7R307022web.jpg</t>
+  </si>
+  <si>
+    <t>7R307014web.jpg</t>
+  </si>
+  <si>
+    <t>7R307013web.jpg</t>
+  </si>
+  <si>
+    <t>7R307012web.jpg</t>
+  </si>
+  <si>
+    <t>7R307006-Editweb.jpg</t>
+  </si>
+  <si>
+    <t>7R306997web.jpg</t>
+  </si>
+  <si>
+    <t>7R306989web.jpg</t>
+  </si>
+  <si>
+    <t>7R306988web.jpg</t>
+  </si>
+  <si>
+    <t>7R306986web.jpg</t>
+  </si>
+  <si>
+    <t>7R306946web.jpg</t>
+  </si>
+  <si>
+    <t>7R306945web.jpg</t>
+  </si>
+  <si>
+    <t>7R306940web.jpg</t>
+  </si>
+  <si>
+    <t>7R306927web.jpg</t>
+  </si>
+  <si>
+    <t>7R306926web.jpg</t>
+  </si>
+  <si>
+    <t>7R306893-Editweb.jpg</t>
+  </si>
+  <si>
+    <t>7R306884web.jpg</t>
+  </si>
+  <si>
+    <t>7R306874web.jpg</t>
+  </si>
+  <si>
+    <t>7R306854web.jpg</t>
+  </si>
+  <si>
+    <t>7R306847web.jpg</t>
+  </si>
+  <si>
+    <t>7R306841web.jpg</t>
+  </si>
+  <si>
+    <t>7R306840web.jpg</t>
+  </si>
+  <si>
+    <t>7R306831web.jpg</t>
+  </si>
+  <si>
+    <t>7R306830web.jpg</t>
+  </si>
+  <si>
+    <t>7R306829web.jpg</t>
+  </si>
+  <si>
+    <t>7R306821web.jpg</t>
+  </si>
+  <si>
+    <t>7R306820web.jpg</t>
+  </si>
+  <si>
+    <t>7R306819web.jpg</t>
+  </si>
+  <si>
+    <t>7R306818web.jpg</t>
+  </si>
+  <si>
+    <t>7R306807web.jpg</t>
+  </si>
+  <si>
+    <t>7R306806web.jpg</t>
+  </si>
+  <si>
+    <t>7R306784web.jpg</t>
+  </si>
+  <si>
+    <t>7R306781web.jpg</t>
+  </si>
+  <si>
+    <t>7R306629web.jpg</t>
+  </si>
+  <si>
+    <t>7R306627web.jpg</t>
+  </si>
+  <si>
+    <t>7R306623web.jpg</t>
+  </si>
+  <si>
+    <t>7R306620web.jpg</t>
+  </si>
+  <si>
+    <t>7R306617web.jpg</t>
+  </si>
+  <si>
+    <t>7R306573web.jpg</t>
+  </si>
+  <si>
+    <t>7R306572web.jpg</t>
+  </si>
+  <si>
+    <t>7R306571web.jpg</t>
+  </si>
+  <si>
+    <t>7R306570web.jpg</t>
+  </si>
+  <si>
+    <t>7R306567web.jpg</t>
+  </si>
+  <si>
+    <t>7R306550-Panoweb.jpg</t>
+  </si>
+  <si>
+    <t>7R306544web.jpg</t>
+  </si>
+  <si>
+    <t>7R306543web.jpg</t>
+  </si>
+  <si>
+    <t>7R306538web.jpg</t>
+  </si>
+  <si>
+    <t>7R306537web.jpg</t>
   </si>
   <si>
     <r>
@@ -282,7 +301,7 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>"images/California</t>
+      <t>"images/Europe/</t>
     </r>
   </si>
   <si>
@@ -305,315 +324,7 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>"Photos from the San Francisco Bay Area."</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF89CA78"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>/&gt;&lt;/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>div</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>&lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFEF596F"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>div</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFBBBBBB"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFD19A66"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>class</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFBBBBBB"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF89CA78"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>"masonryImage"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFBBBBBB"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>&gt; &lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>img</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFBBBBBB"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="7" tint="-0.249977111117893"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>src=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="9" tint="0.39997558519241921"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>"images/Portraits</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>&lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFEF596F"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>div</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFBBBBBB"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFD19A66"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>class</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFBBBBBB"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF89CA78"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>"masonryImage"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFBBBBBB"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>&gt; &lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>img</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFBBBBBB"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="7" tint="-0.249977111117893"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>src=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="9" tint="0.39997558519241921"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>"images/DCNoVA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="7" tint="-0.249977111117893"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>alt=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="9" tint="0.39997558519241921"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>"Photos from DC and the Eastern Shore of Maryland."</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF89CA78"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>/&gt;&lt;/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>div</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="7" tint="-0.249977111117893"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>alt=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="9" tint="0.39997558519241921"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>"Portraits from the San Francisco Bay Area."</t>
+      <t>"Munich, Salzburg, Dolomites, Venice, Trieste"</t>
     </r>
     <r>
       <rPr>
@@ -1023,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43:D52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1042,792 +753,858 @@
     </row>
     <row r="2" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D2" s="3" t="str">
         <f>CONCATENATE(A2,B2,C2)</f>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305417web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306533web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f t="shared" ref="D3:D57" si="0">CONCATENATE(A3,B3,C3)</f>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305592web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <f t="shared" ref="D3:D58" si="0">CONCATENATE(A3,B3,C3)</f>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R307103web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305589web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R307046web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305588-2web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R307044web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305588-1web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R307035web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305587web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R307033web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305586web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R307031-Panoweb.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305585web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R307029web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305579web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R307025web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305578web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R307023web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305566web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R307022web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305564-Panoweb.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R307014web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D14" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305563web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R307013web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D15" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305556web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R307012web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D16" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305554web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R307006-Editweb.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D17" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305552web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306997web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D18" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305544web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306989web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D19" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305543web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306988web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D20" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305522web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306986web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305521web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306946web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D22" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305501web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306945web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D23" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305498web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306940web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D24" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305489web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306927web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D25" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305487web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306926web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D26" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305484web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306893-Editweb.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D27" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305477web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306884web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
         <v>27</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D28" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305476web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306874web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D29" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305474web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306854web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D30" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305470web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306847web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D31" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305467web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306841web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
         <v>31</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D32" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305457web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306840web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
         <v>32</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D33" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305449web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306831web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B34" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D34" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305437web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306830web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B35" t="s">
         <v>34</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D35" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305429web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306829web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B36" t="s">
         <v>35</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D36" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305427web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306821web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B37" t="s">
         <v>36</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D37" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305425web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306820web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B38" t="s">
         <v>37</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D38" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits7R305422web.jpg" alt="Portraits from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306819web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B39" t="s">
         <v>38</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D39" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305248web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306818web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B40" t="s">
         <v>39</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D40" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R305247web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306807web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B41" t="s">
         <v>40</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D41" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R302501web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306806web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B42" t="s">
         <v>41</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D42" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/California7R302498web.jpg" alt="Photos from the San Francisco Bay Area." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306784web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B43" t="s">
         <v>42</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D43" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/DCNoVA7R301870web.jpg" alt="Photos from DC and the Eastern Shore of Maryland." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306781web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B44" t="s">
         <v>43</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D44" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/DCNoVA7R301319web.jpg" alt="Photos from DC and the Eastern Shore of Maryland." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306629web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B45" t="s">
         <v>44</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D45" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/DCNoVA7R301317stackedweb.jpg" alt="Photos from DC and the Eastern Shore of Maryland." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306627web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B46" t="s">
         <v>45</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D46" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/DCNoVA7R300794web.jpg" alt="Photos from DC and the Eastern Shore of Maryland." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306623web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B47" t="s">
         <v>46</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D47" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/DCNoVA7R300790web.jpg" alt="Photos from DC and the Eastern Shore of Maryland." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306620web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B48" t="s">
         <v>47</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D48" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/DCNoVA7R300170web.jpg" alt="Photos from DC and the Eastern Shore of Maryland." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306617web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B49" t="s">
         <v>48</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D49" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/DCNoVA7R300163web.jpg" alt="Photos from DC and the Eastern Shore of Maryland." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306573web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B50" t="s">
         <v>49</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D50" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/DCNoVA7R300162web.jpg" alt="Photos from DC and the Eastern Shore of Maryland." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306572web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B51" t="s">
         <v>50</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D51" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/DCNoVA7R300156web.jpg" alt="Photos from DC and the Eastern Shore of Maryland." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306571web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B52" t="s">
         <v>51</v>
       </c>
       <c r="C52" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D52" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306570web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" t="s">
+        <v>52</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D53" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306567web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54" t="s">
+        <v>53</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D54" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306550-Panoweb.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55" t="s">
+        <v>54</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D55" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306544web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D56" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306543web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" t="s">
         <v>56</v>
       </c>
-      <c r="D52" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/DCNoVA7R300155web.jpg" alt="Photos from DC and the Eastern Shore of Maryland." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="1"/>
-      <c r="C53" s="2"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="1"/>
-      <c r="C54" s="2"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="1"/>
-      <c r="C55" s="2"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="1"/>
-      <c r="C56" s="2"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="1"/>
-      <c r="C57" s="2"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="1"/>
-      <c r="C58" s="2"/>
+      <c r="C57" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D57" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306538web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" t="s">
+        <v>57</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D58" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/7R306537web.jpg" alt="Munich, Salzburg, Dolomites, Venice, Trieste" /&gt;&lt;/div&gt;</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>

</xml_diff>

<commit_message>
Added anemone photos to botanical page
</commit_message>
<xml_diff>
--- a/images/iMaGeUpLoAdErMaGiXpRo.xlsx
+++ b/images/iMaGeUpLoAdErMaGiXpRo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10614"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcamozzo/Desktop/Danny's Stuff/Work/Development/Projects/Photo Website/dcamo001.github.io/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D512536F-B5E3-F546-9157-8D235758BA64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F38FFA-70C0-9F41-A91D-1B6AB4B6703E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28440" windowHeight="22540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10280" yWindow="460" windowWidth="28440" windowHeight="22540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -34,80 +28,121 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>How to use: Paste file names into column B, then copy column D into code</t>
   </si>
   <si>
-    <t>7R307292.jpg</t>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEF596F"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>div</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBBBBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBBBBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF89CA78"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"masonryImage"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBBBBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt; &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>img</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBBBBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7" tint="-0.249977111117893"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>src=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="0.39997558519241921"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"images/Portraits/Devin Murphy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBBBBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>/</t>
+    </r>
   </si>
   <si>
-    <t>7R307278.jpg</t>
+    <t>7R308057web.jpg</t>
   </si>
   <si>
-    <t>7R307285.jpg</t>
+    <t>7R308058web.jpg</t>
   </si>
   <si>
-    <t>7R307288.jpg</t>
-  </si>
-  <si>
-    <t>7R307300.jpg</t>
-  </si>
-  <si>
-    <t>7R307316.jpg</t>
-  </si>
-  <si>
-    <t>7R307323.jpg</t>
-  </si>
-  <si>
-    <t>7R307331.jpg</t>
-  </si>
-  <si>
-    <t>7R307333.jpg</t>
-  </si>
-  <si>
-    <t>7R307348.jpg</t>
-  </si>
-  <si>
-    <t>7R307355.jpg</t>
-  </si>
-  <si>
-    <t>7R307364.jpg</t>
-  </si>
-  <si>
-    <t>7R307366.jpg</t>
-  </si>
-  <si>
-    <t>7R307370.jpg</t>
-  </si>
-  <si>
-    <t>7R307371.jpg</t>
-  </si>
-  <si>
-    <t>7R307373.jpg</t>
-  </si>
-  <si>
-    <t>7R307396.jpg</t>
-  </si>
-  <si>
-    <t>7R307406.jpg</t>
-  </si>
-  <si>
-    <t>7R307415.jpg</t>
-  </si>
-  <si>
-    <t>7R307421.jpg</t>
-  </si>
-  <si>
-    <t>7R307433.jpg</t>
-  </si>
-  <si>
-    <t>7R307435.jpg</t>
-  </si>
-  <si>
-    <t>7R307448.jpg</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">" </t>
     </r>
@@ -127,7 +162,7 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>"Portrait photo session with Devin Murphy, running for Pinole City Council in Pinole, CA."</t>
+      <t>"Giant Green Anemones (Anthopleura xanthogrammica) in Point Reyes, CA, at the South end of Mcclure's Beach."</t>
     </r>
     <r>
       <rPr>
@@ -164,110 +199,6 @@
         <family val="2"/>
       </rPr>
       <t>&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>&lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFEF596F"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>div</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBBBBBB"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD19A66"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>class</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBBBBBB"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF89CA78"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>"masonryImage"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBBBBBB"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>&gt; &lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>img</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBBBBBB"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="7" tint="-0.249977111117893"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>src=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="0.39997558519241921"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>"images/Portraits/Devin Murphy</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBBBBBB"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>/</t>
     </r>
   </si>
 </sst>
@@ -667,7 +598,7 @@
   <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D24"/>
+      <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -686,350 +617,161 @@
       <c r="C1" s="4"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D2" s="5" t="str">
         <f>CONCATENATE(A2,B2,C2)</f>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R307292.jpg" alt="Portrait photo session with Devin Murphy, running for Pinole City Council in Pinole, CA." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R308057web.jpg" alt="Giant Green Anemones (Anthopleura xanthogrammica) in Point Reyes, CA, at the South end of Mcclure's Beach." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D3" s="5" t="str">
         <f t="shared" ref="D3:D24" si="0">CONCATENATE(A3,B3,C3)</f>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R307278.jpg" alt="Portrait photo session with Devin Murphy, running for Pinole City Council in Pinole, CA." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R308058web.jpg" alt="Giant Green Anemones (Anthopleura xanthogrammica) in Point Reyes, CA, at the South end of Mcclure's Beach." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R307285.jpg" alt="Portrait photo session with Devin Murphy, running for Pinole City Council in Pinole, CA." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R307288.jpg" alt="Portrait photo session with Devin Murphy, running for Pinole City Council in Pinole, CA." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R307300.jpg" alt="Portrait photo session with Devin Murphy, running for Pinole City Council in Pinole, CA." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R307316.jpg" alt="Portrait photo session with Devin Murphy, running for Pinole City Council in Pinole, CA." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R307323.jpg" alt="Portrait photo session with Devin Murphy, running for Pinole City Council in Pinole, CA." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R307331.jpg" alt="Portrait photo session with Devin Murphy, running for Pinole City Council in Pinole, CA." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R307333.jpg" alt="Portrait photo session with Devin Murphy, running for Pinole City Council in Pinole, CA." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R307348.jpg" alt="Portrait photo session with Devin Murphy, running for Pinole City Council in Pinole, CA." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R307355.jpg" alt="Portrait photo session with Devin Murphy, running for Pinole City Council in Pinole, CA." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R307364.jpg" alt="Portrait photo session with Devin Murphy, running for Pinole City Council in Pinole, CA." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R307366.jpg" alt="Portrait photo session with Devin Murphy, running for Pinole City Council in Pinole, CA." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R307370.jpg" alt="Portrait photo session with Devin Murphy, running for Pinole City Council in Pinole, CA." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R307371.jpg" alt="Portrait photo session with Devin Murphy, running for Pinole City Council in Pinole, CA." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R307373.jpg" alt="Portrait photo session with Devin Murphy, running for Pinole City Council in Pinole, CA." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R307396.jpg" alt="Portrait photo session with Devin Murphy, running for Pinole City Council in Pinole, CA." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R307406.jpg" alt="Portrait photo session with Devin Murphy, running for Pinole City Council in Pinole, CA." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R307415.jpg" alt="Portrait photo session with Devin Murphy, running for Pinole City Council in Pinole, CA." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R307421.jpg" alt="Portrait photo session with Devin Murphy, running for Pinole City Council in Pinole, CA." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R307433.jpg" alt="Portrait photo session with Devin Murphy, running for Pinole City Council in Pinole, CA." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R307435.jpg" alt="Portrait photo session with Devin Murphy, running for Pinole City Council in Pinole, CA." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R307448.jpg" alt="Portrait photo session with Devin Murphy, running for Pinole City Council in Pinole, CA." /&gt;&lt;/div&gt;</v>
-      </c>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="6"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="6"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="6"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="6"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="6"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="6"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="6"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="6"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="6"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="6"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="6"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="6"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="6"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="6"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="6"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="6"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="6"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="6"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="6"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="6"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>

</xml_diff>

<commit_message>
Updated all albums with new photos, added Styles & Stems album on portraits page
</commit_message>
<xml_diff>
--- a/images/iMaGeUpLoAdErMaGiXpRo.xlsx
+++ b/images/iMaGeUpLoAdErMaGiXpRo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcamozzo/Desktop/Danny's Stuff/Work/Development/Projects/Photo Website/dcamo001.github.io/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F38FFA-70C0-9F41-A91D-1B6AB4B6703E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72F9157-F8E0-3F4F-856C-F2171AA77646}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10280" yWindow="460" windowWidth="28440" windowHeight="22540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11780" yWindow="460" windowWidth="28440" windowHeight="22540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
   <si>
     <t>How to use: Paste file names into column B, then copy column D into code</t>
   </si>
@@ -124,7 +124,7 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>"images/Portraits/Devin Murphy</t>
+      <t>"images</t>
     </r>
     <r>
       <rPr>
@@ -133,14 +133,187 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>/</t>
-    </r>
-  </si>
-  <si>
-    <t>7R308057web.jpg</t>
-  </si>
-  <si>
-    <t>7R308058web.jpg</t>
+      <t>/Portraits/devin murphy</t>
+    </r>
+  </si>
+  <si>
+    <t>7R308565web.jpg</t>
+  </si>
+  <si>
+    <t>7R308569web.jpg</t>
+  </si>
+  <si>
+    <t>7R308576web.jpg</t>
+  </si>
+  <si>
+    <t>7R308577web.jpg</t>
+  </si>
+  <si>
+    <t>7R308599web.jpg</t>
+  </si>
+  <si>
+    <t>7R308607web.jpg</t>
+  </si>
+  <si>
+    <t>7R308609web.jpg</t>
+  </si>
+  <si>
+    <t>7R308620web.jpg</t>
+  </si>
+  <si>
+    <t>7R308634web.jpg</t>
+  </si>
+  <si>
+    <t>7R308641web.jpg</t>
+  </si>
+  <si>
+    <t>7R308644web.jpg</t>
+  </si>
+  <si>
+    <t>7R308648web.jpg</t>
+  </si>
+  <si>
+    <t>7R308660web.jpg</t>
+  </si>
+  <si>
+    <t>7R308677web.jpg</t>
+  </si>
+  <si>
+    <t>7R308685web.jpg</t>
+  </si>
+  <si>
+    <t>7R308718web.jpg</t>
+  </si>
+  <si>
+    <t>7R308719web.jpg</t>
+  </si>
+  <si>
+    <t>7R308725web.jpg</t>
+  </si>
+  <si>
+    <t>7R308770web.jpg</t>
+  </si>
+  <si>
+    <t>7R308787web.jpg</t>
+  </si>
+  <si>
+    <t>7R308791web.jpg</t>
+  </si>
+  <si>
+    <t>7R308798web.jpg</t>
+  </si>
+  <si>
+    <t>7R308807web.jpg</t>
+  </si>
+  <si>
+    <t>7R308813web.jpg</t>
+  </si>
+  <si>
+    <t>7R308817web.jpg</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEF596F"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>div</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBBBBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBBBBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF89CA78"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"masonryImage"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBBBBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt; &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>img</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBBBBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7" tint="-0.249977111117893"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>src=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="0.39997558519241921"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"images</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBBBBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>/StylesandStems/Sept27</t>
+    </r>
   </si>
   <si>
     <r>
@@ -162,7 +335,7 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>"Giant Green Anemones (Anthopleura xanthogrammica) in Point Reyes, CA, at the South end of Mcclure's Beach."</t>
+      <t>"Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020."</t>
     </r>
     <r>
       <rPr>
@@ -189,16 +362,7 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>div</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>&gt;</t>
+      <t>div&gt;</t>
     </r>
   </si>
 </sst>
@@ -598,7 +762,7 @@
   <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D3"/>
+      <selection activeCell="D2" sqref="D2:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -617,19 +781,19 @@
       <c r="C1" s="4"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="D2" s="5" t="str">
         <f>CONCATENATE(A2,B2,C2)</f>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R308057web.jpg" alt="Giant Green Anemones (Anthopleura xanthogrammica) in Point Reyes, CA, at the South end of Mcclure's Beach." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/StylesandStems/Sept277R308565web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="80" x14ac:dyDescent="0.2">
@@ -640,146 +804,357 @@
         <v>3</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="5" t="str">
+        <f t="shared" ref="D3:D26" si="0">CONCATENATE(A3,B3,C3)</f>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/devin murphy7R308569web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="str">
-        <f t="shared" ref="D3:D24" si="0">CONCATENATE(A3,B3,C3)</f>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/Devin Murphy/7R308058web.jpg" alt="Giant Green Anemones (Anthopleura xanthogrammica) in Point Reyes, CA, at the South end of Mcclure's Beach." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="5"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="5"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="5"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="6"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="5"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="6"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="5"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="C26" s="2"/>
+      <c r="C4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/devin murphy7R308576web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/devin murphy7R308577web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/devin murphy7R308599web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/devin murphy7R308607web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/devin murphy7R308609web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/devin murphy7R308620web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/devin murphy7R308634web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/devin murphy7R308641web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/devin murphy7R308644web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/devin murphy7R308648web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/devin murphy7R308660web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/devin murphy7R308677web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/devin murphy7R308685web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/devin murphy7R308718web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/devin murphy7R308719web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/devin murphy7R308725web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/devin murphy7R308770web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/devin murphy7R308787web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/devin murphy7R308791web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/devin murphy7R308798web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/devin murphy7R308807web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/devin murphy7R308813web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/devin murphy7R308817web.jpg" alt="Photos with Leah Nebbett of Styles and Stems. Photographing for Alsace wines in Goat Rock Beach, Jenner, CA on September 27, 2020." /&gt;&lt;/div&gt;</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>

</xml_diff>

<commit_message>
Updated about page photo, added photos to portraits page, added a Design page and removed Karaoke All Stars
</commit_message>
<xml_diff>
--- a/images/iMaGeUpLoAdErMaGiXpRo.xlsx
+++ b/images/iMaGeUpLoAdErMaGiXpRo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcamozzo/Desktop/Danny's Stuff/Work/Development/Projects/Photo Website/dcamo001.github.io/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D7D0E8-CCA8-B24E-9CD6-659CAEE52B99}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEFD60B-C398-5347-AFCC-63975D1767E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28440" windowHeight="22540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3880" yWindow="880" windowWidth="28440" windowHeight="22540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,16 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -28,9 +38,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
   <si>
     <t>How to use: Paste file names into column B, then copy column D into code</t>
+  </si>
+  <si>
+    <t>7R302705.jpg</t>
+  </si>
+  <si>
+    <t>7R302766.jpg</t>
+  </si>
+  <si>
+    <t>7R302764.jpg</t>
+  </si>
+  <si>
+    <t>7R302706.jpg</t>
+  </si>
+  <si>
+    <t>7R302519.jpg</t>
+  </si>
+  <si>
+    <t>7R302495.jpg</t>
+  </si>
+  <si>
+    <t>7R302248.jpg</t>
+  </si>
+  <si>
+    <t>7R302253.jpg</t>
+  </si>
+  <si>
+    <t>7R302255.jpg</t>
+  </si>
+  <si>
+    <t>7R302170.jpg</t>
+  </si>
+  <si>
+    <t>7R302168.jpg</t>
+  </si>
+  <si>
+    <t>7R302154.jpg</t>
   </si>
   <si>
     <r>
@@ -133,56 +179,8 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>/Hawaii/</t>
+      <t>/Portraits/</t>
     </r>
-  </si>
-  <si>
-    <t>7R301112_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301117_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301120_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301151_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301157_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301158_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301160_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301163_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301165-Pano_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301179_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301180_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301190_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301194_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301205_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301208-Pano_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301217_web.jpg</t>
   </si>
   <si>
     <r>
@@ -204,239 +202,7 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>"Photos from Oahu, Hawaii in November of 2021. Photos of North Beach and Banzai Pipeline, Olomana Trail Hike, and more."</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF89CA78"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>/&gt;&lt;/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>div&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>&lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFEF596F"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>div</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBBBBBB"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD19A66"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>class</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBBBBBB"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF89CA78"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>"masonryImage"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBBBBBB"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>&gt; &lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>img</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBBBBBB"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="7" tint="-0.249977111117893"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>src=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="0.39997558519241921"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>"images</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBBBBBB"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>/Celsos/</t>
-    </r>
-  </si>
-  <si>
-    <t>7R301224_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301228_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301232_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301236_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301237_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301238_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301240_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301243_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301244_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301245_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301246_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301250_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301251_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301252_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301255_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301256_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301261_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301262_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301268_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301269_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301272_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301273_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301283_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301284_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301285_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301289_web.jpg</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="7" tint="-0.249977111117893"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>alt=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="0.39997558519241921"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>"Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name."</t>
+      <t>"Photos from Venice, Florence, Tuscany, in Spring of 2022."</t>
     </r>
     <r>
       <rPr>
@@ -846,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D162"/>
+  <dimension ref="A1:D209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -870,633 +636,339 @@
     </row>
     <row r="2" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D2" s="3" t="str">
         <f>CONCATENATE(A2,B2,C2)</f>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Hawaii/7R301112_web.jpg" alt="Photos from Oahu, Hawaii in November of 2021. Photos of North Beach and Banzai Pipeline, Olomana Trail Hike, and more." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R302766.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f t="shared" ref="D3:D18" si="0">CONCATENATE(A3,B3,C3)</f>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Hawaii/7R301117_web.jpg" alt="Photos from Oahu, Hawaii in November of 2021. Photos of North Beach and Banzai Pipeline, Olomana Trail Hike, and more." /&gt;&lt;/div&gt;</v>
+        <f t="shared" ref="D3:D66" si="0">CONCATENATE(A3,B3,C3)</f>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R302764.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Hawaii/7R301120_web.jpg" alt="Photos from Oahu, Hawaii in November of 2021. Photos of North Beach and Banzai Pipeline, Olomana Trail Hike, and more." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R302706.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="C5" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Hawaii/7R301151_web.jpg" alt="Photos from Oahu, Hawaii in November of 2021. Photos of North Beach and Banzai Pipeline, Olomana Trail Hike, and more." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R302705.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Hawaii/7R301157_web.jpg" alt="Photos from Oahu, Hawaii in November of 2021. Photos of North Beach and Banzai Pipeline, Olomana Trail Hike, and more." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R302519.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Hawaii/7R301158_web.jpg" alt="Photos from Oahu, Hawaii in November of 2021. Photos of North Beach and Banzai Pipeline, Olomana Trail Hike, and more." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R302495.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Hawaii/7R301160_web.jpg" alt="Photos from Oahu, Hawaii in November of 2021. Photos of North Beach and Banzai Pipeline, Olomana Trail Hike, and more." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R302248.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Hawaii/7R301163_web.jpg" alt="Photos from Oahu, Hawaii in November of 2021. Photos of North Beach and Banzai Pipeline, Olomana Trail Hike, and more." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R302253.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Hawaii/7R301165-Pano_web.jpg" alt="Photos from Oahu, Hawaii in November of 2021. Photos of North Beach and Banzai Pipeline, Olomana Trail Hike, and more." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R302255.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Hawaii/7R301179_web.jpg" alt="Photos from Oahu, Hawaii in November of 2021. Photos of North Beach and Banzai Pipeline, Olomana Trail Hike, and more." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R302170.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Hawaii/7R301180_web.jpg" alt="Photos from Oahu, Hawaii in November of 2021. Photos of North Beach and Banzai Pipeline, Olomana Trail Hike, and more." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R302168.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Hawaii/7R301190_web.jpg" alt="Photos from Oahu, Hawaii in November of 2021. Photos of North Beach and Banzai Pipeline, Olomana Trail Hike, and more." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Hawaii/7R301194_web.jpg" alt="Photos from Oahu, Hawaii in November of 2021. Photos of North Beach and Banzai Pipeline, Olomana Trail Hike, and more." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Hawaii/7R301205_web.jpg" alt="Photos from Oahu, Hawaii in November of 2021. Photos of North Beach and Banzai Pipeline, Olomana Trail Hike, and more." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Hawaii/7R301208-Pano_web.jpg" alt="Photos from Oahu, Hawaii in November of 2021. Photos of North Beach and Banzai Pipeline, Olomana Trail Hike, and more." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Hawaii/7R301217_web.jpg" alt="Photos from Oahu, Hawaii in November of 2021. Photos of North Beach and Banzai Pipeline, Olomana Trail Hike, and more." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301224_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="3" t="str">
-        <f t="shared" ref="D19:D43" si="1">CONCATENATE(A19,B19,C19)</f>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301228_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301232_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301236_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301237_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301238_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301240_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301243_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301244_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301245_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301246_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D29" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301250_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301251_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301252_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301255_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B33" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301256_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B34" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D34" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301261_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D35" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301262_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D36" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301268_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B37" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D37" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301269_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D38" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301272_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B39" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301273_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B40" t="s">
-        <v>42</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D40" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301283_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" t="s">
-        <v>43</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D41" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301284_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" t="s">
-        <v>44</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D42" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301285_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B43" t="s">
-        <v>45</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D43" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301289_web.jpg" alt="Photos from Celsos Hair and Beard in Alameda, California. Local high quality barbershop with a great story behind the name." /&gt;&lt;/div&gt;</v>
-      </c>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R302154.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="4"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="4"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="4"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="4"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="4"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="4"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="4"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="4"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="4"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="4"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="4"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="4"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="4"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="4"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
@@ -2093,6 +1565,241 @@
       <c r="C162" s="5"/>
       <c r="D162" s="3"/>
     </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163" s="4"/>
+      <c r="C163" s="5"/>
+      <c r="D163" s="3"/>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164" s="4"/>
+      <c r="C164" s="5"/>
+      <c r="D164" s="3"/>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A165" s="4"/>
+      <c r="C165" s="5"/>
+      <c r="D165" s="3"/>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A166" s="4"/>
+      <c r="C166" s="5"/>
+      <c r="D166" s="3"/>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A167" s="4"/>
+      <c r="C167" s="5"/>
+      <c r="D167" s="3"/>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A168" s="4"/>
+      <c r="C168" s="5"/>
+      <c r="D168" s="3"/>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A169" s="4"/>
+      <c r="C169" s="5"/>
+      <c r="D169" s="3"/>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A170" s="4"/>
+      <c r="C170" s="5"/>
+      <c r="D170" s="3"/>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A171" s="4"/>
+      <c r="C171" s="5"/>
+      <c r="D171" s="3"/>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A172" s="4"/>
+      <c r="C172" s="5"/>
+      <c r="D172" s="3"/>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A173" s="4"/>
+      <c r="C173" s="5"/>
+      <c r="D173" s="3"/>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A174" s="4"/>
+      <c r="C174" s="5"/>
+      <c r="D174" s="3"/>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A175" s="4"/>
+      <c r="C175" s="5"/>
+      <c r="D175" s="3"/>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A176" s="4"/>
+      <c r="C176" s="5"/>
+      <c r="D176" s="3"/>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A177" s="4"/>
+      <c r="C177" s="5"/>
+      <c r="D177" s="3"/>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A178" s="4"/>
+      <c r="C178" s="5"/>
+      <c r="D178" s="3"/>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A179" s="4"/>
+      <c r="C179" s="5"/>
+      <c r="D179" s="3"/>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A180" s="4"/>
+      <c r="C180" s="5"/>
+      <c r="D180" s="3"/>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A181" s="4"/>
+      <c r="C181" s="5"/>
+      <c r="D181" s="3"/>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A182" s="4"/>
+      <c r="C182" s="5"/>
+      <c r="D182" s="3"/>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A183" s="4"/>
+      <c r="C183" s="5"/>
+      <c r="D183" s="3"/>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A184" s="4"/>
+      <c r="C184" s="5"/>
+      <c r="D184" s="3"/>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A185" s="4"/>
+      <c r="C185" s="5"/>
+      <c r="D185" s="3"/>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A186" s="4"/>
+      <c r="C186" s="5"/>
+      <c r="D186" s="3"/>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A187" s="4"/>
+      <c r="C187" s="5"/>
+      <c r="D187" s="3"/>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A188" s="4"/>
+      <c r="C188" s="5"/>
+      <c r="D188" s="3"/>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A189" s="4"/>
+      <c r="C189" s="5"/>
+      <c r="D189" s="3"/>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A190" s="4"/>
+      <c r="C190" s="5"/>
+      <c r="D190" s="3"/>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A191" s="4"/>
+      <c r="C191" s="5"/>
+      <c r="D191" s="3"/>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A192" s="4"/>
+      <c r="C192" s="5"/>
+      <c r="D192" s="3"/>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A193" s="4"/>
+      <c r="C193" s="5"/>
+      <c r="D193" s="3"/>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A194" s="4"/>
+      <c r="C194" s="5"/>
+      <c r="D194" s="3"/>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A195" s="4"/>
+      <c r="C195" s="5"/>
+      <c r="D195" s="3"/>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A196" s="4"/>
+      <c r="C196" s="5"/>
+      <c r="D196" s="3"/>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A197" s="4"/>
+      <c r="C197" s="5"/>
+      <c r="D197" s="3"/>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A198" s="4"/>
+      <c r="C198" s="5"/>
+      <c r="D198" s="3"/>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A199" s="4"/>
+      <c r="C199" s="5"/>
+      <c r="D199" s="3"/>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A200" s="4"/>
+      <c r="C200" s="5"/>
+      <c r="D200" s="3"/>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A201" s="4"/>
+      <c r="C201" s="5"/>
+      <c r="D201" s="3"/>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A202" s="4"/>
+      <c r="C202" s="5"/>
+      <c r="D202" s="3"/>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A203" s="4"/>
+      <c r="C203" s="5"/>
+      <c r="D203" s="3"/>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A204" s="4"/>
+      <c r="C204" s="5"/>
+      <c r="D204" s="3"/>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A205" s="4"/>
+      <c r="C205" s="5"/>
+      <c r="D205" s="3"/>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A206" s="4"/>
+      <c r="C206" s="5"/>
+      <c r="D206" s="3"/>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A207" s="4"/>
+      <c r="C207" s="5"/>
+      <c r="D207" s="3"/>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A208" s="4"/>
+      <c r="C208" s="5"/>
+      <c r="D208" s="3"/>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A209" s="4"/>
+      <c r="C209" s="5"/>
+      <c r="D209" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finished all updates for now. Small update to prints page, new photo on about page, added Design album, added photos to Flora, Portraits, and Europe albums.
</commit_message>
<xml_diff>
--- a/images/iMaGeUpLoAdErMaGiXpRo.xlsx
+++ b/images/iMaGeUpLoAdErMaGiXpRo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcamozzo/Desktop/Danny's Stuff/Work/Development/Projects/Photo Website/dcamo001.github.io/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEFD60B-C398-5347-AFCC-63975D1767E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A9A2FD-1324-E44A-9E21-08EF08348AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3880" yWindow="880" windowWidth="28440" windowHeight="22540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,45 +38,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>How to use: Paste file names into column B, then copy column D into code</t>
   </si>
   <si>
-    <t>7R302705.jpg</t>
+    <t>7R301261_web.jpg</t>
   </si>
   <si>
-    <t>7R302766.jpg</t>
+    <t>7R301251_web.jpg</t>
   </si>
   <si>
-    <t>7R302764.jpg</t>
+    <t>7R301238_web.jpg</t>
   </si>
   <si>
-    <t>7R302706.jpg</t>
+    <t>7R301237_web.jpg</t>
   </si>
   <si>
-    <t>7R302519.jpg</t>
-  </si>
-  <si>
-    <t>7R302495.jpg</t>
-  </si>
-  <si>
-    <t>7R302248.jpg</t>
-  </si>
-  <si>
-    <t>7R302253.jpg</t>
-  </si>
-  <si>
-    <t>7R302255.jpg</t>
-  </si>
-  <si>
-    <t>7R302170.jpg</t>
-  </si>
-  <si>
-    <t>7R302168.jpg</t>
-  </si>
-  <si>
-    <t>7R302154.jpg</t>
+    <t>7R301236_web.jpg</t>
   </si>
   <si>
     <r>
@@ -179,7 +158,7 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>/Portraits/</t>
+      <t>/Celsos/</t>
     </r>
   </si>
   <si>
@@ -202,7 +181,7 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>"Photos from Venice, Florence, Tuscany, in Spring of 2022."</t>
+      <t>"Interior design shots from Ceslsos Hair and Beard in Alameda, California."</t>
     </r>
     <r>
       <rPr>
@@ -615,7 +594,7 @@
   <dimension ref="A1:D209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D13"/>
+      <selection activeCell="D2" sqref="D2:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -634,185 +613,122 @@
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D2" s="3" t="str">
         <f>CONCATENATE(A2,B2,C2)</f>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R302766.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301261_web.jpg" alt="Interior design shots from Ceslsos Hair and Beard in Alameda, California." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="str">
+        <f t="shared" ref="D3:D39" si="0">CONCATENATE(A3,B3,C3)</f>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301251_web.jpg" alt="Interior design shots from Ceslsos Hair and Beard in Alameda, California." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3" t="str">
-        <f t="shared" ref="D3:D66" si="0">CONCATENATE(A3,B3,C3)</f>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R302764.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="C4" s="5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R302706.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301238_web.jpg" alt="Interior design shots from Ceslsos Hair and Beard in Alameda, California." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R302705.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301237_web.jpg" alt="Interior design shots from Ceslsos Hair and Beard in Alameda, California." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R302519.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R302495.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R302248.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R302253.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R302255.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R302170.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R302168.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R302154.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301236_web.jpg" alt="Interior design shots from Ceslsos Hair and Beard in Alameda, California." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
@@ -945,10 +861,13 @@
       <c r="C38" s="5"/>
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="C39" s="5"/>
-      <c r="D39" s="3"/>
+      <c r="D39" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>

</xml_diff>

<commit_message>
Added Mavic photos to the Italy album
</commit_message>
<xml_diff>
--- a/images/iMaGeUpLoAdErMaGiXpRo.xlsx
+++ b/images/iMaGeUpLoAdErMaGiXpRo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcamozzo/Desktop/Danny's Stuff/Work/Development/Projects/Photo Website/dcamo001.github.io/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A9A2FD-1324-E44A-9E21-08EF08348AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063246B8-892A-E041-BAE3-3EA3C197C9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3880" yWindow="880" windowWidth="28440" windowHeight="22540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,24 +38,120 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="40">
   <si>
     <t>How to use: Paste file names into column B, then copy column D into code</t>
   </si>
   <si>
-    <t>7R301261_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301251_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301238_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301237_web.jpg</t>
-  </si>
-  <si>
-    <t>7R301236_web.jpg</t>
+    <t>7R301810web.jpg</t>
+  </si>
+  <si>
+    <t>7R301814web.jpg</t>
+  </si>
+  <si>
+    <t>7R301824web.jpg</t>
+  </si>
+  <si>
+    <t>7R302020web.jpg</t>
+  </si>
+  <si>
+    <t>7R302145web.jpg</t>
+  </si>
+  <si>
+    <t>7R302184web.jpg</t>
+  </si>
+  <si>
+    <t>7R302192web.jpg</t>
+  </si>
+  <si>
+    <t>7R302471web.jpg</t>
+  </si>
+  <si>
+    <t>7R302472web.jpg</t>
+  </si>
+  <si>
+    <t>7R302530web.jpg</t>
+  </si>
+  <si>
+    <t>7R302532web.jpg</t>
+  </si>
+  <si>
+    <t>7R302647web.jpg</t>
+  </si>
+  <si>
+    <t>7R302665web.jpg</t>
+  </si>
+  <si>
+    <t>7R302720web.jpg</t>
+  </si>
+  <si>
+    <t>7R302802web.jpg</t>
+  </si>
+  <si>
+    <t>7R302803web.jpg</t>
+  </si>
+  <si>
+    <t>7R302804web.jpg</t>
+  </si>
+  <si>
+    <t>7R302805web.jpg</t>
+  </si>
+  <si>
+    <t>7R302806web.jpg</t>
+  </si>
+  <si>
+    <t>7R303077web.jpg</t>
+  </si>
+  <si>
+    <t>7R303078web.jpg</t>
+  </si>
+  <si>
+    <t>7R303079web.jpg</t>
+  </si>
+  <si>
+    <t>7R303081web.jpg</t>
+  </si>
+  <si>
+    <t>7R303082web.jpg</t>
+  </si>
+  <si>
+    <t>7R303083web.jpg</t>
+  </si>
+  <si>
+    <t>7R303084web.jpg</t>
+  </si>
+  <si>
+    <t>7R303181web.jpg</t>
+  </si>
+  <si>
+    <t>7R302494web.jpg</t>
+  </si>
+  <si>
+    <t>7R302500web.jpg</t>
+  </si>
+  <si>
+    <t>7R302501web.jpg</t>
+  </si>
+  <si>
+    <t>7R302503web.jpg</t>
+  </si>
+  <si>
+    <t>7R302511web.jpg</t>
+  </si>
+  <si>
+    <t>7R302661web.jpg</t>
+  </si>
+  <si>
+    <t>7R303179web.jpg</t>
+  </si>
+  <si>
+    <t>7R303180web.jpg</t>
+  </si>
+  <si>
+    <t>7R303227web.jpg</t>
+  </si>
+  <si>
+    <t>7R303231web.jpg</t>
   </si>
   <si>
     <r>
@@ -158,7 +254,7 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>/Celsos/</t>
+      <t>/Design/</t>
     </r>
   </si>
   <si>
@@ -181,7 +277,7 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>"Interior design shots from Ceslsos Hair and Beard in Alameda, California."</t>
+      <t>"Photos from Venice, Florence, Tuscany, in Spring of 2022."</t>
     </r>
     <r>
       <rPr>
@@ -591,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D209"/>
+  <dimension ref="A1:D210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D6"/>
+      <selection activeCell="D2" sqref="D2:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -613,261 +709,565 @@
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="D2" s="3" t="str">
         <f>CONCATENATE(A2,B2,C2)</f>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301261_web.jpg" alt="Interior design shots from Ceslsos Hair and Beard in Alameda, California." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R301810web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f t="shared" ref="D3:D39" si="0">CONCATENATE(A3,B3,C3)</f>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301251_web.jpg" alt="Interior design shots from Ceslsos Hair and Beard in Alameda, California." /&gt;&lt;/div&gt;</v>
+        <f t="shared" ref="D3:D66" si="0">CONCATENATE(A3,B3,C3)</f>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R301814web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="D4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301238_web.jpg" alt="Interior design shots from Ceslsos Hair and Beard in Alameda, California." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R301824web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="D5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301237_web.jpg" alt="Interior design shots from Ceslsos Hair and Beard in Alameda, California." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302020web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302145web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302184web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Celsos/7R301236_web.jpg" alt="Interior design shots from Ceslsos Hair and Beard in Alameda, California." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="4"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="4"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="4"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="4"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="C8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302192web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302471web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302472web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302494web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302500web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302501web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302503web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302511web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302530web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302532web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302647web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302661web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302665web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302720web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302802web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302803web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302804web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302805web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302806web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R303077web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R303078web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R303079web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R303081web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R303082web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R303083web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R303084web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R303179web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R303180web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R303181web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R303227web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R303231web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="C39" s="5"/>
-      <c r="D39" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
@@ -1719,6 +2119,11 @@
       <c r="C209" s="5"/>
       <c r="D209" s="3"/>
     </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A210" s="4"/>
+      <c r="C210" s="5"/>
+      <c r="D210" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed title of Europe page, re ordered people and things index page for mobile
</commit_message>
<xml_diff>
--- a/images/iMaGeUpLoAdErMaGiXpRo.xlsx
+++ b/images/iMaGeUpLoAdErMaGiXpRo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcamozzo/Desktop/Danny's Stuff/Work/Development/Projects/Photo Website/dcamo001.github.io/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063246B8-892A-E041-BAE3-3EA3C197C9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085BE887-623B-194D-AEDB-3BC6A186D95A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3880" yWindow="880" windowWidth="28440" windowHeight="22540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,120 +38,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="13">
   <si>
     <t>How to use: Paste file names into column B, then copy column D into code</t>
   </si>
   <si>
-    <t>7R301810web.jpg</t>
+    <t>DJI_0157web.jpg</t>
   </si>
   <si>
-    <t>7R301814web.jpg</t>
+    <t>DJI_0160web.jpg</t>
   </si>
   <si>
-    <t>7R301824web.jpg</t>
+    <t>DJI_0163web.jpg</t>
   </si>
   <si>
-    <t>7R302020web.jpg</t>
+    <t>DJI_0167web.jpg</t>
   </si>
   <si>
-    <t>7R302145web.jpg</t>
+    <t>DJI_0173web.jpg</t>
   </si>
   <si>
-    <t>7R302184web.jpg</t>
+    <t>DJI_0176web.jpg</t>
   </si>
   <si>
-    <t>7R302192web.jpg</t>
+    <t>DJI_0178web.jpg</t>
   </si>
   <si>
-    <t>7R302471web.jpg</t>
+    <t>DJI_0181web.jpg</t>
   </si>
   <si>
-    <t>7R302472web.jpg</t>
+    <t>DJI_0191web.jpg</t>
   </si>
   <si>
-    <t>7R302530web.jpg</t>
-  </si>
-  <si>
-    <t>7R302532web.jpg</t>
-  </si>
-  <si>
-    <t>7R302647web.jpg</t>
-  </si>
-  <si>
-    <t>7R302665web.jpg</t>
-  </si>
-  <si>
-    <t>7R302720web.jpg</t>
-  </si>
-  <si>
-    <t>7R302802web.jpg</t>
-  </si>
-  <si>
-    <t>7R302803web.jpg</t>
-  </si>
-  <si>
-    <t>7R302804web.jpg</t>
-  </si>
-  <si>
-    <t>7R302805web.jpg</t>
-  </si>
-  <si>
-    <t>7R302806web.jpg</t>
-  </si>
-  <si>
-    <t>7R303077web.jpg</t>
-  </si>
-  <si>
-    <t>7R303078web.jpg</t>
-  </si>
-  <si>
-    <t>7R303079web.jpg</t>
-  </si>
-  <si>
-    <t>7R303081web.jpg</t>
-  </si>
-  <si>
-    <t>7R303082web.jpg</t>
-  </si>
-  <si>
-    <t>7R303083web.jpg</t>
-  </si>
-  <si>
-    <t>7R303084web.jpg</t>
-  </si>
-  <si>
-    <t>7R303181web.jpg</t>
-  </si>
-  <si>
-    <t>7R302494web.jpg</t>
-  </si>
-  <si>
-    <t>7R302500web.jpg</t>
-  </si>
-  <si>
-    <t>7R302501web.jpg</t>
-  </si>
-  <si>
-    <t>7R302503web.jpg</t>
-  </si>
-  <si>
-    <t>7R302511web.jpg</t>
-  </si>
-  <si>
-    <t>7R302661web.jpg</t>
-  </si>
-  <si>
-    <t>7R303179web.jpg</t>
-  </si>
-  <si>
-    <t>7R303180web.jpg</t>
-  </si>
-  <si>
-    <t>7R303227web.jpg</t>
-  </si>
-  <si>
-    <t>7R303231web.jpg</t>
+    <t>DJI_0195web.jpg</t>
   </si>
   <si>
     <r>
@@ -254,7 +173,7 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>/Design/</t>
+      <t>/Europe/Italy Spring 2022/Mavic</t>
     </r>
   </si>
   <si>
@@ -277,7 +196,7 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>"Photos from Venice, Florence, Tuscany, in Spring of 2022."</t>
+      <t>"Photos from Florence, Lupaia in Tuscany, and Cinque Terre in Spring of 2022."</t>
     </r>
     <r>
       <rPr>
@@ -690,7 +609,7 @@
   <dimension ref="A1:D210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D38"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -709,560 +628,298 @@
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D2" s="3" t="str">
         <f>CONCATENATE(A2,B2,C2)</f>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R301810web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/Italy Spring 2022/MavicDJI_0157web.jpg" alt="Photos from Florence, Lupaia in Tuscany, and Cinque Terre in Spring of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f t="shared" ref="D3:D66" si="0">CONCATENATE(A3,B3,C3)</f>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R301814web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+        <f t="shared" ref="D3:D38" si="0">CONCATENATE(A3,B3,C3)</f>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/Italy Spring 2022/MavicDJI_0160web.jpg" alt="Photos from Florence, Lupaia in Tuscany, and Cinque Terre in Spring of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R301824web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/Italy Spring 2022/MavicDJI_0163web.jpg" alt="Photos from Florence, Lupaia in Tuscany, and Cinque Terre in Spring of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302020web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/Italy Spring 2022/MavicDJI_0167web.jpg" alt="Photos from Florence, Lupaia in Tuscany, and Cinque Terre in Spring of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302145web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/Italy Spring 2022/MavicDJI_0173web.jpg" alt="Photos from Florence, Lupaia in Tuscany, and Cinque Terre in Spring of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302184web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/Italy Spring 2022/MavicDJI_0176web.jpg" alt="Photos from Florence, Lupaia in Tuscany, and Cinque Terre in Spring of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302192web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/Italy Spring 2022/MavicDJI_0178web.jpg" alt="Photos from Florence, Lupaia in Tuscany, and Cinque Terre in Spring of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302471web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/Italy Spring 2022/MavicDJI_0181web.jpg" alt="Photos from Florence, Lupaia in Tuscany, and Cinque Terre in Spring of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302472web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/Italy Spring 2022/MavicDJI_0191web.jpg" alt="Photos from Florence, Lupaia in Tuscany, and Cinque Terre in Spring of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302494web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302500web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302501web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302503web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302511web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302530web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302532web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302647web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302661web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302665web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302720web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302802web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302803web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302804web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302805web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R302806web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R303077web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R303078web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R303079web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B30" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R303081web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R303082web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R303083web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D33" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R303084web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D34" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R303179web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D35" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R303180web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" t="s">
-        <v>27</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R303181web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" t="s">
-        <v>36</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D37" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R303227web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" t="s">
-        <v>37</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D38" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Design/7R303231web.jpg" alt="Photos from Venice, Florence, Tuscany, in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/Italy Spring 2022/MavicDJI_0195web.jpg" alt="Photos from Florence, Lupaia in Tuscany, and Cinque Terre in Spring of 2022." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="4"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="4"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="4"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="4"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="4"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="4"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="4"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="4"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="4"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="4"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>

</xml_diff>

<commit_message>
added photos from crab feast and Summer trip east, some reorganization
</commit_message>
<xml_diff>
--- a/images/iMaGeUpLoAdErMaGiXpRo.xlsx
+++ b/images/iMaGeUpLoAdErMaGiXpRo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcamozzo/Desktop/Danny's Stuff/Work/Development/Projects/Photo Website/dcamo001.github.io/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085BE887-623B-194D-AEDB-3BC6A186D95A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B44075-38A4-3B40-B9AF-B8BDEEE32BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3880" yWindow="880" windowWidth="28440" windowHeight="22540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="23900" windowHeight="20900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,39 +38,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="20">
   <si>
     <t>How to use: Paste file names into column B, then copy column D into code</t>
   </si>
   <si>
-    <t>DJI_0157web.jpg</t>
-  </si>
-  <si>
-    <t>DJI_0160web.jpg</t>
-  </si>
-  <si>
-    <t>DJI_0163web.jpg</t>
-  </si>
-  <si>
-    <t>DJI_0167web.jpg</t>
-  </si>
-  <si>
-    <t>DJI_0173web.jpg</t>
-  </si>
-  <si>
-    <t>DJI_0176web.jpg</t>
-  </si>
-  <si>
-    <t>DJI_0178web.jpg</t>
-  </si>
-  <si>
-    <t>DJI_0181web.jpg</t>
-  </si>
-  <si>
-    <t>DJI_0191web.jpg</t>
-  </si>
-  <si>
-    <t>DJI_0195web.jpg</t>
+    <t>7R303401web.jpg</t>
+  </si>
+  <si>
+    <t>7R303404web.jpg</t>
+  </si>
+  <si>
+    <t>7R303447web.jpg</t>
+  </si>
+  <si>
+    <t>7R303448web.jpg</t>
+  </si>
+  <si>
+    <t>7R303474web.jpg</t>
+  </si>
+  <si>
+    <t>7R303477web.jpg</t>
+  </si>
+  <si>
+    <t>7R303478web.jpg</t>
+  </si>
+  <si>
+    <t>7R303503web.jpg</t>
+  </si>
+  <si>
+    <t>7R303508web.jpg</t>
+  </si>
+  <si>
+    <t>7R303527web.jpg</t>
+  </si>
+  <si>
+    <t>7R303545web.jpg</t>
+  </si>
+  <si>
+    <t>7R303559web.jpg</t>
+  </si>
+  <si>
+    <t>7R303575web.jpg</t>
+  </si>
+  <si>
+    <t>7R303664web.jpg</t>
+  </si>
+  <si>
+    <t>7R303695web.jpg</t>
+  </si>
+  <si>
+    <t>7R303704web.jpg</t>
+  </si>
+  <si>
+    <t>7R303716web.jpg</t>
   </si>
   <si>
     <r>
@@ -173,7 +194,7 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>/Europe/Italy Spring 2022/Mavic</t>
+      <t>/Portraits/</t>
     </r>
   </si>
   <si>
@@ -196,7 +217,7 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>"Photos from Florence, Lupaia in Tuscany, and Cinque Terre in Spring of 2022."</t>
+      <t>"Photos of friends on top of Mt Tamalpais, and in Berkeley California."</t>
     </r>
     <r>
       <rPr>
@@ -608,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D210"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -630,195 +651,258 @@
     </row>
     <row r="2" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D2" s="3" t="str">
         <f>CONCATENATE(A2,B2,C2)</f>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/Italy Spring 2022/MavicDJI_0157web.jpg" alt="Photos from Florence, Lupaia in Tuscany, and Cinque Terre in Spring of 2022." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303401web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f t="shared" ref="D3:D38" si="0">CONCATENATE(A3,B3,C3)</f>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/Italy Spring 2022/MavicDJI_0160web.jpg" alt="Photos from Florence, Lupaia in Tuscany, and Cinque Terre in Spring of 2022." /&gt;&lt;/div&gt;</v>
+        <f t="shared" ref="D3:D29" si="0">CONCATENATE(A3,B3,C3)</f>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303404web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/Italy Spring 2022/MavicDJI_0163web.jpg" alt="Photos from Florence, Lupaia in Tuscany, and Cinque Terre in Spring of 2022." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303447web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/Italy Spring 2022/MavicDJI_0167web.jpg" alt="Photos from Florence, Lupaia in Tuscany, and Cinque Terre in Spring of 2022." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303448web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/Italy Spring 2022/MavicDJI_0173web.jpg" alt="Photos from Florence, Lupaia in Tuscany, and Cinque Terre in Spring of 2022." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303474web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/Italy Spring 2022/MavicDJI_0176web.jpg" alt="Photos from Florence, Lupaia in Tuscany, and Cinque Terre in Spring of 2022." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303477web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/Italy Spring 2022/MavicDJI_0178web.jpg" alt="Photos from Florence, Lupaia in Tuscany, and Cinque Terre in Spring of 2022." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303478web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/Italy Spring 2022/MavicDJI_0181web.jpg" alt="Photos from Florence, Lupaia in Tuscany, and Cinque Terre in Spring of 2022." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303503web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/Italy Spring 2022/MavicDJI_0191web.jpg" alt="Photos from Florence, Lupaia in Tuscany, and Cinque Terre in Spring of 2022." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303508web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Europe/Italy Spring 2022/MavicDJI_0195web.jpg" alt="Photos from Florence, Lupaia in Tuscany, and Cinque Terre in Spring of 2022." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="3"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303527web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303545web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303559web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303575web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303664web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303695web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303704web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303716web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>

</xml_diff>

<commit_message>
New photos since June 2022 until now, some homepage reorganization
</commit_message>
<xml_diff>
--- a/images/iMaGeUpLoAdErMaGiXpRo.xlsx
+++ b/images/iMaGeUpLoAdErMaGiXpRo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcamozzo/Desktop/Danny's Stuff/Work/Development/Projects/Photo Website/dcamo001.github.io/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B44075-38A4-3B40-B9AF-B8BDEEE32BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E1C9EE-29CB-DC4B-9576-77B8B1ED3532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="23900" windowHeight="20900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,136 +38,229 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>How to use: Paste file names into column B, then copy column D into code</t>
   </si>
   <si>
-    <t>7R303401web.jpg</t>
+    <t>DSCF0846-Editweb.jpg</t>
   </si>
   <si>
-    <t>7R303404web.jpg</t>
+    <t>DSCF0851web.jpg</t>
   </si>
   <si>
-    <t>7R303447web.jpg</t>
+    <t>DSCF1302web.jpg</t>
   </si>
   <si>
-    <t>7R303448web.jpg</t>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFEF596F"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>div</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBBBBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD19A66"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBBBBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF89CA78"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"masonryImage"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBBBBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt; &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>img</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBBBBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7" tint="-0.249977111117893"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>src=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="0.39997558519241921"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"images</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBBBBB"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>/Pretty Things/</t>
+    </r>
   </si>
   <si>
-    <t>7R303474web.jpg</t>
+    <r>
+      <t xml:space="preserve">" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7" tint="-0.249977111117893"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>alt=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="0.39997558519241921"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Photos from California during Winter 2022 and Summer 2023."</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF89CA78"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>/&gt;&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>div&gt;</t>
+    </r>
   </si>
   <si>
-    <t>7R303477web.jpg</t>
+    <t>DSCF3793web.jpg</t>
   </si>
   <si>
-    <t>7R303478web.jpg</t>
+    <r>
+      <t xml:space="preserve">" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="7" tint="-0.249977111117893"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>alt=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="0.39997558519241921"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>"Fall colors in Great Barrington Massachussets in Fall of 2022."</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF89CA78"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>/&gt;&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>div&gt;</t>
+    </r>
   </si>
   <si>
-    <t>7R303503web.jpg</t>
-  </si>
-  <si>
-    <t>7R303508web.jpg</t>
-  </si>
-  <si>
-    <t>7R303527web.jpg</t>
-  </si>
-  <si>
-    <t>7R303545web.jpg</t>
-  </si>
-  <si>
-    <t>7R303559web.jpg</t>
-  </si>
-  <si>
-    <t>7R303575web.jpg</t>
-  </si>
-  <si>
-    <t>7R303664web.jpg</t>
-  </si>
-  <si>
-    <t>7R303695web.jpg</t>
-  </si>
-  <si>
-    <t>7R303704web.jpg</t>
-  </si>
-  <si>
-    <t>7R303716web.jpg</t>
-  </si>
-  <si>
-    <r>
-      <t>&lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFEF596F"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>div</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBBBBBB"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFD19A66"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>class</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBBBBBB"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF89CA78"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>"masonryImage"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBBBBBB"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>&gt; &lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>img</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBBBBBB"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+    <r>
+      <t xml:space="preserve">" </t>
     </r>
     <r>
       <rPr>
@@ -176,7 +269,7 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>src=</t>
+      <t>alt=</t>
     </r>
     <r>
       <rPr>
@@ -185,39 +278,7 @@
         <rFont val="Menlo"/>
         <family val="2"/>
       </rPr>
-      <t>"images</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBBBBBB"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>/Portraits/</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">" </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="7" tint="-0.249977111117893"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>alt=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="0.39997558519241921"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>"Photos of friends on top of Mt Tamalpais, and in Berkeley California."</t>
+      <t>"Fall colors on a winding road in Great Barrington Massachussets in Fall of 2022."</t>
     </r>
     <r>
       <rPr>
@@ -627,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D210"/>
+  <dimension ref="A1:D260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -651,258 +712,141 @@
     </row>
     <row r="2" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D2" s="3" t="str">
         <f>CONCATENATE(A2,B2,C2)</f>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303401web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Pretty Things/DSCF0846-Editweb.jpg" alt="Fall colors in Great Barrington Massachussets in Fall of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f t="shared" ref="D3:D29" si="0">CONCATENATE(A3,B3,C3)</f>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303404web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
+        <f t="shared" ref="D3:D7" si="0">CONCATENATE(A3,B3,C3)</f>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Pretty Things/DSCF0851web.jpg" alt="Fall colors on a winding road in Great Barrington Massachussets in Fall of 2022." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303447web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Pretty Things/DSCF1302web.jpg" alt="Photos from California during Winter 2022 and Summer 2023." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303448web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
+        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Pretty Things/DSCF3793web.jpg" alt="Photos from California during Winter 2022 and Summer 2023." /&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303474web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303477web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303478web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303503web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303508web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303527web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303545web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303559web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303575web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303664web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303695web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303704web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;div class="masonryImage"&gt; &lt;img src="images/Portraits/7R303716web.jpg" alt="Photos of friends on top of Mt Tamalpais, and in Berkeley California." /&gt;&lt;/div&gt;</v>
-      </c>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
@@ -1865,6 +1809,256 @@
       <c r="C210" s="5"/>
       <c r="D210" s="3"/>
     </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A211" s="4"/>
+      <c r="C211" s="5"/>
+      <c r="D211" s="3"/>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A212" s="4"/>
+      <c r="C212" s="5"/>
+      <c r="D212" s="3"/>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A213" s="4"/>
+      <c r="C213" s="5"/>
+      <c r="D213" s="3"/>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A214" s="4"/>
+      <c r="C214" s="5"/>
+      <c r="D214" s="3"/>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A215" s="4"/>
+      <c r="C215" s="5"/>
+      <c r="D215" s="3"/>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A216" s="4"/>
+      <c r="C216" s="5"/>
+      <c r="D216" s="3"/>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A217" s="4"/>
+      <c r="C217" s="5"/>
+      <c r="D217" s="3"/>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A218" s="4"/>
+      <c r="C218" s="5"/>
+      <c r="D218" s="3"/>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A219" s="4"/>
+      <c r="C219" s="5"/>
+      <c r="D219" s="3"/>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A220" s="4"/>
+      <c r="C220" s="5"/>
+      <c r="D220" s="3"/>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A221" s="4"/>
+      <c r="C221" s="5"/>
+      <c r="D221" s="3"/>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A222" s="4"/>
+      <c r="C222" s="5"/>
+      <c r="D222" s="3"/>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A223" s="4"/>
+      <c r="C223" s="5"/>
+      <c r="D223" s="3"/>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A224" s="4"/>
+      <c r="C224" s="5"/>
+      <c r="D224" s="3"/>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A225" s="4"/>
+      <c r="C225" s="5"/>
+      <c r="D225" s="3"/>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A226" s="4"/>
+      <c r="C226" s="5"/>
+      <c r="D226" s="3"/>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A227" s="4"/>
+      <c r="C227" s="5"/>
+      <c r="D227" s="3"/>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A228" s="4"/>
+      <c r="C228" s="5"/>
+      <c r="D228" s="3"/>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A229" s="4"/>
+      <c r="C229" s="5"/>
+      <c r="D229" s="3"/>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A230" s="4"/>
+      <c r="C230" s="5"/>
+      <c r="D230" s="3"/>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A231" s="4"/>
+      <c r="C231" s="5"/>
+      <c r="D231" s="3"/>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A232" s="4"/>
+      <c r="C232" s="5"/>
+      <c r="D232" s="3"/>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A233" s="4"/>
+      <c r="C233" s="5"/>
+      <c r="D233" s="3"/>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A234" s="4"/>
+      <c r="C234" s="5"/>
+      <c r="D234" s="3"/>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A235" s="4"/>
+      <c r="C235" s="5"/>
+      <c r="D235" s="3"/>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A236" s="4"/>
+      <c r="C236" s="5"/>
+      <c r="D236" s="3"/>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A237" s="4"/>
+      <c r="C237" s="5"/>
+      <c r="D237" s="3"/>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A238" s="4"/>
+      <c r="C238" s="5"/>
+      <c r="D238" s="3"/>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A239" s="4"/>
+      <c r="C239" s="5"/>
+      <c r="D239" s="3"/>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A240" s="4"/>
+      <c r="C240" s="5"/>
+      <c r="D240" s="3"/>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A241" s="4"/>
+      <c r="C241" s="5"/>
+      <c r="D241" s="3"/>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A242" s="4"/>
+      <c r="C242" s="5"/>
+      <c r="D242" s="3"/>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A243" s="4"/>
+      <c r="C243" s="5"/>
+      <c r="D243" s="3"/>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A244" s="4"/>
+      <c r="C244" s="5"/>
+      <c r="D244" s="3"/>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A245" s="4"/>
+      <c r="C245" s="5"/>
+      <c r="D245" s="3"/>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A246" s="4"/>
+      <c r="C246" s="5"/>
+      <c r="D246" s="3"/>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A247" s="4"/>
+      <c r="C247" s="5"/>
+      <c r="D247" s="3"/>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A248" s="4"/>
+      <c r="C248" s="5"/>
+      <c r="D248" s="3"/>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A249" s="4"/>
+      <c r="C249" s="5"/>
+      <c r="D249" s="3"/>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A250" s="4"/>
+      <c r="C250" s="5"/>
+      <c r="D250" s="3"/>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A251" s="4"/>
+      <c r="C251" s="5"/>
+      <c r="D251" s="3"/>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A252" s="4"/>
+      <c r="C252" s="5"/>
+      <c r="D252" s="3"/>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A253" s="4"/>
+      <c r="C253" s="5"/>
+      <c r="D253" s="3"/>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A254" s="4"/>
+      <c r="C254" s="5"/>
+      <c r="D254" s="3"/>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A255" s="4"/>
+      <c r="C255" s="5"/>
+      <c r="D255" s="3"/>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A256" s="4"/>
+      <c r="C256" s="5"/>
+      <c r="D256" s="3"/>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A257" s="4"/>
+      <c r="C257" s="5"/>
+      <c r="D257" s="3"/>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A258" s="4"/>
+      <c r="C258" s="5"/>
+      <c r="D258" s="3"/>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A259" s="4"/>
+      <c r="C259" s="5"/>
+      <c r="D259" s="3"/>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A260" s="4"/>
+      <c r="C260" s="5"/>
+      <c r="D260" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>